<commit_message>
Fix xlsx file & refactor item_type check
</commit_message>
<xml_diff>
--- a/excel/brief_example_gi3.xlsx
+++ b/excel/brief_example_gi3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZhernokE\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A23585-CFBE-4F3D-87E5-ACF05F1F0B05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA6D64F-A403-48AB-B4FF-A2966E5D8FEE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D56199A6-23DC-9C48-9AED-27640EB21542}"/>
+    <workbookView xWindow="90" yWindow="375" windowWidth="20400" windowHeight="10800" xr2:uid="{D56199A6-23DC-9C48-9AED-27640EB21542}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="196">
   <si>
     <t>FSC</t>
   </si>
@@ -592,9 +592,6 @@
   </si>
   <si>
     <t xml:space="preserve">Набор "Мерцание глаз" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pазмер </t>
   </si>
   <si>
     <t>6 (16-16,5 мм)</t>
@@ -1382,8 +1379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BBE2B86-7C91-E04C-83EE-E98EF11EDA0F}">
   <dimension ref="A1:S95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
@@ -1498,7 +1495,7 @@
     </row>
     <row r="5" spans="1:19" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A5" s="26" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:19" s="60" customFormat="1" ht="21" customHeight="1">
@@ -1607,7 +1604,7 @@
         <v>41</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E11" s="35" t="s">
         <v>168</v>
@@ -1639,7 +1636,7 @@
         <v>43</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E12" s="35" t="s">
         <v>168</v>
@@ -1671,7 +1668,7 @@
         <v>45</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>168</v>
@@ -1703,7 +1700,7 @@
         <v>46</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E14" s="35" t="s">
         <v>168</v>
@@ -1735,10 +1732,10 @@
         <v>48</v>
       </c>
       <c r="D15" s="35" t="s">
+        <v>179</v>
+      </c>
+      <c r="E15" s="35" t="s">
         <v>180</v>
-      </c>
-      <c r="E15" s="35" t="s">
-        <v>181</v>
       </c>
       <c r="F15" s="46" t="s">
         <v>169</v>
@@ -1767,10 +1764,10 @@
         <v>49</v>
       </c>
       <c r="D16" s="35" t="s">
+        <v>179</v>
+      </c>
+      <c r="E16" s="35" t="s">
         <v>180</v>
-      </c>
-      <c r="E16" s="35" t="s">
-        <v>181</v>
       </c>
       <c r="F16" s="46" t="s">
         <v>169</v>
@@ -1799,10 +1796,10 @@
         <v>50</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E17" s="35" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F17" s="46" t="s">
         <v>169</v>
@@ -1922,7 +1919,7 @@
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B24" s="37"/>
       <c r="C24" s="37"/>
@@ -1944,7 +1941,7 @@
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="38" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -2310,7 +2307,7 @@
     </row>
     <row r="44" spans="1:16" s="1" customFormat="1" ht="15" customHeight="1">
       <c r="A44" s="26" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B44" s="2"/>
     </row>
@@ -2355,10 +2352,10 @@
         <v>1234568</v>
       </c>
       <c r="D47" s="84" t="s">
+        <v>184</v>
+      </c>
+      <c r="E47" s="84" t="s">
         <v>185</v>
-      </c>
-      <c r="E47" s="84" t="s">
-        <v>186</v>
       </c>
       <c r="F47" s="66"/>
       <c r="K47" s="77">
@@ -2374,10 +2371,10 @@
         <v>1234569</v>
       </c>
       <c r="D48" s="85" t="s">
+        <v>186</v>
+      </c>
+      <c r="E48" s="66" t="s">
         <v>187</v>
-      </c>
-      <c r="E48" s="66" t="s">
-        <v>188</v>
       </c>
       <c r="F48" s="66"/>
       <c r="G48" s="66"/>
@@ -2393,10 +2390,10 @@
         <v>1234560</v>
       </c>
       <c r="D49" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="E49" s="86" t="s">
         <v>189</v>
-      </c>
-      <c r="E49" s="86" t="s">
-        <v>190</v>
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
@@ -2413,10 +2410,10 @@
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="86" t="s">
+        <v>190</v>
+      </c>
+      <c r="E50" s="86" t="s">
         <v>191</v>
-      </c>
-      <c r="E50" s="86" t="s">
-        <v>192</v>
       </c>
       <c r="G50" s="3"/>
       <c r="K50" s="76">
@@ -2450,7 +2447,7 @@
     </row>
     <row r="53" spans="1:16" s="1" customFormat="1" ht="15" customHeight="1">
       <c r="A53" s="26" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B53" s="2"/>
     </row>
@@ -2548,16 +2545,16 @@
         <v>123789</v>
       </c>
       <c r="D58" s="28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E58" s="66" t="s">
         <v>96</v>
       </c>
       <c r="F58" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="G58" s="66" t="s">
         <v>173</v>
-      </c>
-      <c r="G58" s="66" t="s">
-        <v>174</v>
       </c>
       <c r="K58" s="66">
         <v>400</v>
@@ -2571,16 +2568,16 @@
         <v>123789</v>
       </c>
       <c r="D59" s="28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E59" s="66" t="s">
         <v>96</v>
       </c>
       <c r="F59" s="25" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G59" s="66" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K59" s="66">
         <v>400</v>
@@ -2594,16 +2591,16 @@
         <v>123789</v>
       </c>
       <c r="D60" s="28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E60" s="66" t="s">
         <v>96</v>
       </c>
       <c r="F60" s="25" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G60" s="66" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K60" s="66">
         <v>400</v>
@@ -2827,7 +2824,7 @@
     </row>
     <row r="72" spans="1:13" s="87" customFormat="1" ht="27" customHeight="1">
       <c r="A72" s="87" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D72" s="88"/>
       <c r="E72" s="88"/>
@@ -2841,7 +2838,7 @@
     </row>
     <row r="73" spans="1:13" s="81" customFormat="1" ht="27" customHeight="1">
       <c r="A73" s="81" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D73" s="82"/>
       <c r="E73" s="82"/>
@@ -3261,7 +3258,7 @@
     </row>
     <row r="88" spans="1:13" s="87" customFormat="1" ht="27" customHeight="1">
       <c r="A88" s="87" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D88" s="88"/>
       <c r="E88" s="88"/>
@@ -3275,7 +3272,7 @@
     </row>
     <row r="89" spans="1:13" s="81" customFormat="1" ht="27" customHeight="1">
       <c r="A89" s="81" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D89" s="82"/>
       <c r="E89" s="82"/>
@@ -3304,7 +3301,7 @@
         <v>158</v>
       </c>
       <c r="F90" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G90" s="10" t="s">
         <v>163</v>
@@ -3336,7 +3333,7 @@
         <v>35</v>
       </c>
       <c r="F91" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G91" s="10" t="s">
         <v>164</v>
@@ -3368,7 +3365,7 @@
         <v>35</v>
       </c>
       <c r="F92" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G92" s="10" t="s">
         <v>165</v>
@@ -3400,7 +3397,7 @@
         <v>161</v>
       </c>
       <c r="F93" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G93" s="10" t="s">
         <v>166</v>
@@ -3432,7 +3429,7 @@
         <v>161</v>
       </c>
       <c r="F94" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G94" s="10" t="s">
         <v>165</v>
@@ -3464,7 +3461,7 @@
         <v>161</v>
       </c>
       <c r="F95" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G95" s="10" t="s">
         <v>167</v>

</xml_diff>